<commit_message>
need to rerun power n1 to include pre-contingency loadings.
</commit_message>
<xml_diff>
--- a/model_outputs/analysis_power_contingency/excel_branch_response.xlsx
+++ b/model_outputs/analysis_power_contingency/excel_branch_response.xlsx
@@ -39,16 +39,16 @@
     <t>Average error</t>
   </si>
   <si>
-    <t>Post-contingency</t>
+    <t>maximum</t>
   </si>
   <si>
-    <t>Post-response</t>
+    <t>Longest response time</t>
   </si>
   <si>
-    <t>Longest response</t>
+    <t>Post-contingency loading</t>
   </si>
   <si>
-    <t>maximum</t>
+    <t>Post-response loading</t>
   </si>
 </sst>
 </file>
@@ -638,7 +638,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Longest response</c:v>
+                  <c:v>Longest response time</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3705,7 +3705,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Post-contingency</c:v>
+                  <c:v>Post-contingency loading</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6762,7 +6762,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Post-response</c:v>
+                  <c:v>Post-response loading</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -14224,8 +14224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J502"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -14238,13 +14238,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>1</v>
@@ -14262,7 +14262,7 @@
         <v>5</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">

</xml_diff>